<commit_message>
update new modules about microbiome 16S pipeline
</commit_message>
<xml_diff>
--- a/data/HRSD/Metadata_HRSD.xlsx
+++ b/data/HRSD/Metadata_HRSD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/yy663_cornell_edu/Documents/2021 postdoc/3-WERF-short cut nitrification-Jangho/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zijianleowang/Desktop/GitHub/EasyMicrobiome/data/HRSD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{543B63AB-E43D-4D06-B947-9CF9930306C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D59838FB-A93F-4B89-BE1B-247142EEE5B7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB168C8-B75D-AA47-86B5-F9CCAE8FEDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="1236" windowWidth="23256" windowHeight="12456" xr2:uid="{2A956713-CEF3-4FC3-AA81-251CE4FF0127}"/>
+    <workbookView xWindow="5540" yWindow="1240" windowWidth="23260" windowHeight="12460" xr2:uid="{2A956713-CEF3-4FC3-AA81-251CE4FF0127}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Day</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>VFA to SBPR category</t>
+  </si>
+  <si>
+    <t>Sample name</t>
   </si>
 </sst>
 </file>
@@ -138,67 +141,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <color theme="0"/>
@@ -572,15 +515,18 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="15" width="9.140625" style="1"/>
+    <col min="3" max="15" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>190703</v>
       </c>
@@ -666,7 +612,7 @@
         <v>0.17199999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>190802</v>
       </c>
@@ -714,7 +660,7 @@
         <v>0.19700000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>190830</v>
       </c>
@@ -762,7 +708,7 @@
         <v>0.41099999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>190913</v>
       </c>
@@ -810,7 +756,7 @@
         <v>0.46800000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>191004</v>
       </c>
@@ -852,7 +798,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>191019</v>
       </c>
@@ -894,7 +840,7 @@
         <v>0.995</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>191025</v>
       </c>
@@ -942,7 +888,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>191108</v>
       </c>
@@ -990,7 +936,7 @@
         <v>2.21</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>191111</v>
       </c>
@@ -1032,7 +978,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>191115</v>
       </c>
@@ -1080,7 +1026,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>191122</v>
       </c>
@@ -1125,7 +1071,7 @@
         <v>3.3960413542279211</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>191129</v>
       </c>
@@ -1167,7 +1113,7 @@
         <v>2.84</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>191206</v>
       </c>
@@ -1215,7 +1161,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>191213</v>
       </c>
@@ -1257,7 +1203,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>191220</v>
       </c>
@@ -1305,7 +1251,7 @@
         <v>6.62</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>200103</v>
       </c>
@@ -1347,7 +1293,7 @@
         <v>6.4</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>200110</v>
       </c>
@@ -1395,7 +1341,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>200117</v>
       </c>
@@ -1443,7 +1389,7 @@
         <v>4.43</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>200124</v>
       </c>
@@ -1491,7 +1437,7 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>200131</v>
       </c>
@@ -1539,7 +1485,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>200205</v>
       </c>

</xml_diff>